<commit_message>
Next time sheet boiii
</commit_message>
<xml_diff>
--- a/Admin/Gaby/TimeSheet_Week12.xlsx
+++ b/Admin/Gaby/TimeSheet_Week12.xlsx
@@ -361,10 +361,10 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="2" style="0" width="6.5"/>
@@ -586,12 +586,16 @@
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
+      <c r="F13" s="10" t="n">
+        <v>2</v>
+      </c>
       <c r="G13" s="11"/>
-      <c r="H13" s="10"/>
+      <c r="H13" s="10" t="n">
+        <v>4</v>
+      </c>
       <c r="I13" s="12" t="n">
         <f aca="false">SUM(B13:H13)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J13" s="8"/>
     </row>
@@ -617,7 +621,7 @@
       </c>
       <c r="F14" s="12" t="n">
         <f aca="false">SUM(F6:F13)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G14" s="12" t="n">
         <f aca="false">SUM(G6:G13)</f>
@@ -625,11 +629,11 @@
       </c>
       <c r="H14" s="12" t="n">
         <f aca="false">SUM(H6:H13)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I14" s="12" t="n">
         <f aca="false">SUM(I6:I13)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>